<commit_message>
Zmieniony teleport marker i usuniete zbedne prefaby
</commit_message>
<xml_diff>
--- a/License.xlsx
+++ b/License.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152F356F-8ED5-413F-99FC-F902E7331A6B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B38949-50E8-4C67-A42B-DEA0FAC56CB7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22259" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>https://assetstore.unity.com/packages/tools/integration/oculus-integration-82022</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>https://assetstore.unity.com/packages/templates/tutorials/oculus-sample-framework-82503</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/models/d39c906029df4837a9a0538cbbacd234</t>
   </si>
 </sst>
 </file>
@@ -314,16 +317,16 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -608,7 +611,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.25"/>
@@ -617,211 +620,213 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K18" t="s">
@@ -829,7 +834,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K19" t="s">
@@ -848,19 +853,20 @@
     <mergeCell ref="A10:J10"/>
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A6:J6"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A4:J4"/>
     <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A6:J6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{C98DC073-9C4D-4294-B114-CC4F0E2F4574}"/>
     <hyperlink ref="K17" r:id="rId2" xr:uid="{5A2D1593-A492-487C-988D-B24EABCEF2CA}"/>
     <hyperlink ref="A2" r:id="rId3" xr:uid="{1CF3241D-65AA-4E46-A6B7-1E9AA233534D}"/>
+    <hyperlink ref="A3" r:id="rId4" xr:uid="{12572346-4843-446B-85F9-3858A95725D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId4"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Improved Menu and scripts
</commit_message>
<xml_diff>
--- a/License.xlsx
+++ b/License.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B38949-50E8-4C67-A42B-DEA0FAC56CB7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8CA045-B8F8-4B1B-80DA-FF6DF8FF5A14}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22259" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>https://assetstore.unity.com/packages/tools/integration/oculus-integration-82022</t>
   </si>
@@ -250,6 +250,15 @@
   </si>
   <si>
     <t>https://sketchfab.com/models/d39c906029df4837a9a0538cbbacd234</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;Icons made by &lt;a href="https://www.flaticon.com/authors/gregor-cresnar" title="Gregor Cresnar"&gt;Gregor Cresnar&lt;/a&gt; from &lt;a href="https://www.flaticon.com/" 			    title="Flaticon"&gt;www.flaticon.com&lt;/a&gt; is licensed by &lt;a href="http://creativecommons.org/licenses/by/3.0/" 			    title="Creative Commons BY 3.0" target="_blank"&gt;CC 3.0 BY&lt;/a&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>@</t>
   </si>
 </sst>
 </file>
@@ -611,15 +620,16 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="10" max="10" width="63.25" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -633,7 +643,7 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -647,7 +657,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -661,8 +671,10 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -672,9 +684,14 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="K4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -684,9 +701,14 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="K5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -697,7 +719,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -709,7 +731,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -721,7 +743,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -733,7 +755,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -745,7 +767,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -757,7 +779,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -769,7 +791,7 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -781,7 +803,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -793,7 +815,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -805,7 +827,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -843,6 +865,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A14:J14"/>
     <mergeCell ref="A15:J15"/>
@@ -853,12 +881,6 @@
     <mergeCell ref="A10:J10"/>
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A12:J12"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A5:J5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{C98DC073-9C4D-4294-B114-CC4F0E2F4574}"/>

</xml_diff>

<commit_message>
Added hand and fixed UI
</commit_message>
<xml_diff>
--- a/License.xlsx
+++ b/License.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B762440D-1DAF-4BAB-AEDB-77241BDCB34A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB9CAFD-95F3-45DD-88D8-CD136C936F7E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22259" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>https://assetstore.unity.com/packages/tools/integration/oculus-integration-82022</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>@</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/models/d30eff5c6082446a8adfc7ccfe938873</t>
   </si>
 </sst>
 </file>
@@ -620,7 +623,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:J12"/>
+      <selection activeCell="A7" sqref="A7:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.25"/>
@@ -720,7 +723,9 @@
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -865,12 +870,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A14:J14"/>
     <mergeCell ref="A15:J15"/>
@@ -881,14 +880,21 @@
     <mergeCell ref="A10:J10"/>
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:J5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{C98DC073-9C4D-4294-B114-CC4F0E2F4574}"/>
     <hyperlink ref="K17" r:id="rId2" xr:uid="{5A2D1593-A492-487C-988D-B24EABCEF2CA}"/>
     <hyperlink ref="A2" r:id="rId3" xr:uid="{1CF3241D-65AA-4E46-A6B7-1E9AA233534D}"/>
     <hyperlink ref="A3" r:id="rId4" xr:uid="{12572346-4843-446B-85F9-3858A95725D6}"/>
+    <hyperlink ref="A7" r:id="rId5" xr:uid="{4A2C5AE4-3FCB-478B-84DA-01B4FD10D8F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made chain in Maya Working fifth riddle (some bug exists) To fix(longer chains,distant of each sack;) Some other bugs exists but i couldnt recreate them Added fifth number to password !!! Game almost completed !!!
</commit_message>
<xml_diff>
--- a/License.xlsx
+++ b/License.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEDFC9D-7438-4EA1-BB5C-6060E0AB1480}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22259" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>https://assetstore.unity.com/packages/tools/integration/oculus-integration-82022</t>
   </si>
@@ -271,12 +270,57 @@
   </si>
   <si>
     <t>ADDED</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/models/f0a9b718935f410ba1a8ad0bbf3a7c8a?fbclid=IwAR1SthItjKWBKzIIDFLBxuDhrcEouyK0DfTN5nJrMckN6ikcNl2hK4AQb80</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/models/30afc4aa500a4d06a0101da8740495db?fbclid=IwAR3PImKCWH8r8L7ikl_K-pJsfyOc42CekwmxR8L-C54camnM13OQRpUOm0M</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/models/e64bf63834274acd9efabc2d675fd5c2</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/models/f2656927d6994722bd5a84d364928eb2</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/models/4c32fc04e7a3413b96e56d48618ca484</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/models/7c2f7989d7c54a7188a4e0a4f30a3faa</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/models/db4f3adce26742fca58b11b2bffe4a89</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/models/f34129e40344442691af165f0a833cc5</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/models/faad524e8d5940d99ce7ae96c9a0c18e</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/models/59408c5ce18940fbb903fe946663e2f8</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/models/fc2c7bee06ec42178c97f712f1142cf3</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/models/1f5aefe94e5543969fb0889074c194df</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/models/02aa0965cc9f42cbbc0e70a5811c3a34</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/models/af199ff482b24def9e8216d318c39a79</t>
+  </si>
+  <si>
+    <t>https://sketchfab.com/models/81cee3ac55ce4a77bcfb3b5f3f53a2d8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -343,21 +387,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -634,77 +678,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="38.375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="78.7109375" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" ht="14.1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:12" ht="14.1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" ht="14.1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
       <c r="L3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:12" ht="14.1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
       <c r="K4" t="s">
         <v>9</v>
       </c>
@@ -712,19 +757,19 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:12" ht="14.1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
       <c r="K5" t="s">
         <v>10</v>
       </c>
@@ -732,190 +777,238 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="6" customFormat="1" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="L6" s="6" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="L6" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:12" ht="14.1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
       <c r="L7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:12" ht="14.1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
       <c r="L8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:12" ht="14.1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
       <c r="L9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="A12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+      <c r="A13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="A14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="A15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="A16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="J17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K28" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K29" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K30" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A5:J5"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A14:J14"/>
     <mergeCell ref="A15:J15"/>
@@ -926,17 +1019,30 @@
     <mergeCell ref="A10:J10"/>
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:J5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{C98DC073-9C4D-4294-B114-CC4F0E2F4574}"/>
-    <hyperlink ref="K17" r:id="rId2" xr:uid="{5A2D1593-A492-487C-988D-B24EABCEF2CA}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{1CF3241D-65AA-4E46-A6B7-1E9AA233534D}"/>
-    <hyperlink ref="A3" r:id="rId4" xr:uid="{12572346-4843-446B-85F9-3858A95725D6}"/>
-    <hyperlink ref="A7" r:id="rId5" xr:uid="{4A2C5AE4-3FCB-478B-84DA-01B4FD10D8F8}"/>
-    <hyperlink ref="A8" r:id="rId6" location="download" xr:uid="{2FD2543B-445B-470A-9F88-0ED2FC227482}"/>
-    <hyperlink ref="A9" r:id="rId7" xr:uid="{67011A69-73F0-4582-97FF-7EAF008852F5}"/>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="K28" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="A3" r:id="rId4"/>
+    <hyperlink ref="A7" r:id="rId5"/>
+    <hyperlink ref="A8" r:id="rId6" location="download"/>
+    <hyperlink ref="A9" r:id="rId7"/>
+    <hyperlink ref="A10" r:id="rId8"/>
+    <hyperlink ref="A11" r:id="rId9"/>
+    <hyperlink ref="A12" r:id="rId10"/>
+    <hyperlink ref="A13" r:id="rId11"/>
+    <hyperlink ref="A14" r:id="rId12"/>
+    <hyperlink ref="A15" r:id="rId13"/>
+    <hyperlink ref="A16" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>